<commit_message>
adding MIN_TIMES to excel example (sheet B)
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="88">
   <si>
     <t xml:space="preserve">LIST</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">#B_SAME_ORDERS_IN_ALL_ROUNDS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MIN_TIMES</t>
   </si>
   <si>
     <t xml:space="preserve">Sur une échelle de 1 (pas bénéfiques) à 5 (très bénéfiques), pensez-vous que les Associations Reconnues d’Utilité Publique (ARUP) sont généralement bénéfiques pour la société ?</t>
@@ -393,7 +396,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -501,20 +504,23 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K24"/>
+  <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L5" activeCellId="0" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="45.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="15.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="68.47"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.51"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="29.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="68.11"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="24.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="0" width="17.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="34.05"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -551,28 +557,31 @@
       <c r="K1" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="L1" s="0" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="E2" s="1" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>24</v>
@@ -583,31 +592,34 @@
       <c r="K2" s="1" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="L2" s="0" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="E3" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>38</v>
+      <c r="F3" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>25</v>
@@ -615,362 +627,369 @@
       <c r="J3" s="1" t="n">
         <v>0</v>
       </c>
+      <c r="L3" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="E4" s="1" t="n">
         <v>10</v>
       </c>
+      <c r="F4" s="2"/>
       <c r="G4" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>45</v>
+      <c r="F5" s="2" t="s">
+        <v>46</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>50</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B13" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>68</v>
-      </c>
       <c r="G13" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B16" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>74</v>
-      </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B17" s="1" t="s">
-        <v>76</v>
-      </c>
       <c r="C17" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="2" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -995,11 +1014,11 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
min and max values may change in OPTS for int, float and slider types if both are non empty (for positive values OPTS should always start by :0)
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" state="visible" r:id="rId2"/>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">slider:int</t>
   </si>
   <si>
-    <t xml:space="preserve">99:18:1:17</t>
+    <t xml:space="preserve">99:18:1:18</t>
   </si>
   <si>
     <t xml:space="preserve">age</t>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">Quel est votre genre ?</t>
   </si>
   <si>
-    <t xml:space="preserve">radio:optional</t>
+    <t xml:space="preserve">hradio:optional</t>
   </si>
   <si>
     <t xml:space="preserve">Homme:Femme</t>
@@ -414,14 +414,15 @@
   </sheetPr>
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -518,13 +519,13 @@
       <c r="A7" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
     </row>
@@ -546,7 +547,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -600,7 +601,7 @@
       <c r="L1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M1" s="0" t="s">
+      <c r="M1" s="1" t="s">
         <v>35</v>
       </c>
     </row>
@@ -638,7 +639,7 @@
       <c r="L2" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="M2" s="0" t="n">
+      <c r="M2" s="1" t="n">
         <v>0</v>
       </c>
     </row>
@@ -676,7 +677,7 @@
       <c r="L3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="M3" s="0" t="n">
+      <c r="M3" s="1" t="n">
         <v>1</v>
       </c>
     </row>
@@ -706,7 +707,7 @@
       <c r="L4" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="M4" s="0" t="n">
+      <c r="M4" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
adding more examples, debugging optional slider, adding strip() for options and types
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
   <si>
     <t xml:space="preserve">LIST</t>
   </si>
@@ -78,10 +78,10 @@
     <t xml:space="preserve">Quel est votre genre ?</t>
   </si>
   <si>
-    <t xml:space="preserve">hradio:optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homme:Femme</t>
+    <t xml:space="preserve">hradio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homme:Femme:Je ne veux pas répondre</t>
   </si>
   <si>
     <t xml:space="preserve">genre</t>
@@ -109,6 +109,18 @@
   </si>
   <si>
     <t xml:space="preserve">taille_foyer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question optionnelle : quel pourcentage de vos revenus épargnez-vous chaque mois environ ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">slider:float:optional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:100:0.01:inv:%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">epargne_pourc</t>
   </si>
   <si>
     <t xml:space="preserve">ASSO_LIST</t>
@@ -412,17 +424,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -527,6 +540,20 @@
       </c>
       <c r="D7" s="1" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -547,7 +574,7 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -584,51 +611,51 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>1</v>
@@ -645,31 +672,31 @@
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>40</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>12</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -683,26 +710,26 @@
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>44</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>10</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>0</v>
@@ -713,336 +740,336 @@
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>74</v>
+        <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>77</v>
+        <v>81</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>80</v>
+        <v>84</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>82</v>
+        <v>86</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>81</v>
-      </c>
       <c r="D18" s="2" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="B20" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>83</v>
-      </c>
       <c r="C20" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>88</v>
+        <v>92</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>90</v>
+        <v>94</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>83</v>
+        <v>87</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>91</v>
+        <v>95</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>96</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1071,7 +1098,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changing step ins slider:float example
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -117,7 +117,7 @@
     <t xml:space="preserve">slider:float:optional</t>
   </si>
   <si>
-    <t xml:space="preserve">0:100:0.01:inv:%</t>
+    <t xml:space="preserve">0:100:0.1:inv:%</t>
   </si>
   <si>
     <t xml:space="preserve">epargne_pourc</t>
@@ -433,9 +433,9 @@
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="13.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -552,7 +552,7 @@
       <c r="C8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding vertical slider option
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -114,10 +114,10 @@
     <t xml:space="preserve">Question optionnelle : quel pourcentage de vos revenus épargnez-vous chaque mois environ ?</t>
   </si>
   <si>
-    <t xml:space="preserve">slider:float:optional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0:100:0.1:inv:%</t>
+    <t xml:space="preserve">slider:float:optional:vertical/350</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0:100:0.1:inv:%:Rien du tout/Tout le revenu:0,5,10,15,20,25,30,35,40,45,50,55,60,65,70,75,80,85,90,95,100/1</t>
   </si>
   <si>
     <t xml:space="preserve">epargne_pourc</t>
@@ -426,14 +426,14 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="46.54"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.75"/>
   </cols>

</xml_diff>

<commit_message>
possibility to add px to vertical slider height
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -114,7 +114,7 @@
     <t xml:space="preserve">Question optionnelle : quel pourcentage de vos revenus épargnez-vous chaque mois environ ?</t>
   </si>
   <si>
-    <t xml:space="preserve">slider:float:optional:vertical/350</t>
+    <t xml:space="preserve">slider:float:optional:vertical/350px</t>
   </si>
   <si>
     <t xml:space="preserve">0:100:0.1:inv:%:Rien du tout/Tout le revenu:0,5,10,15,20,25,30,35,40,45,50,55,60,65,70,75,80,85,90,95,100/1</t>
@@ -426,7 +426,7 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adding HASTAG aprameter - for indicating that tag in questions shoudl be taken into account and QUESTTAG parameter - to change the default tag (H5) in non single-line and non radiotable questions
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="101">
   <si>
     <t xml:space="preserve">LIST</t>
   </si>
@@ -42,6 +42,12 @@
     <t xml:space="preserve">BY_INTRO</t>
   </si>
   <si>
+    <t xml:space="preserve">HASTAGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QUESTTAG</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quel âge avez-vous ?</t>
   </si>
   <si>
@@ -81,12 +87,15 @@
     <t xml:space="preserve">hradio</t>
   </si>
   <si>
-    <t xml:space="preserve">Homme:Femme:Je ne veux pas répondre</t>
+    <t xml:space="preserve">Homme:Femme:Je ne veux &lt;b&gt;&lt;u&gt;pas&lt;/u&gt;&lt;/b&gt; répondre</t>
   </si>
   <si>
     <t xml:space="preserve">genre</t>
   </si>
   <si>
+    <t xml:space="preserve">div style='font-size:120%'</t>
+  </si>
+  <si>
     <t xml:space="preserve">Quel est votre pays de naissance?</t>
   </si>
   <si>
@@ -99,7 +108,35 @@
     <t xml:space="preserve">pays</t>
   </si>
   <si>
-    <t xml:space="preserve">De combien de personnes votre foyer est-il composé ?</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">De combien de &lt;u&gt;&lt;b&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <u val="single"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">personnes</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;/b&gt;&lt;/u&gt; votre foyer est-il composé ?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">int</t>
@@ -322,10 +359,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -346,6 +384,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <u val="single"/>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -390,7 +436,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -400,6 +446,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -424,10 +474,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -457,19 +507,25 @@
       <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>0</v>
@@ -477,83 +533,93 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
+      </c>
+      <c r="H5" s="0" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>32</v>
+        <v>35</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -611,51 +677,51 @@
         <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
-        <v>40</v>
+      <c r="A2" s="4" t="s">
+        <v>43</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="E2" s="2" t="n">
         <v>1</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J2" s="2" t="n">
         <v>1</v>
@@ -671,32 +737,32 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3" t="s">
-        <v>46</v>
+      <c r="A3" s="4" t="s">
+        <v>49</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>44</v>
       </c>
       <c r="E3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>49</v>
+      <c r="F3" s="4" t="s">
+        <v>52</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="J3" s="2" t="n">
         <v>0</v>
@@ -709,27 +775,27 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3" t="s">
-        <v>52</v>
+      <c r="A4" s="4" t="s">
+        <v>55</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="E4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="3"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="2" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>0</v>
@@ -739,337 +805,337 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
-        <v>55</v>
+      <c r="A5" s="4" t="s">
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="2" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D17" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H5" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" s="2" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="H6" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="H7" s="2" t="s">
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D19" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="H8" s="2" t="s">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D20" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" s="2" t="s">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="2" t="s">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H11" s="2" t="s">
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D23" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D24" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C13" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D18" s="2" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B24" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1098,7 +1164,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updating README, deleting extra space in the example questionnaire
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -8,9 +8,9 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="A" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="B" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="#C" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="A" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="B" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="#C" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -78,7 +78,7 @@
     <t xml:space="preserve">diplome</t>
   </si>
   <si>
-    <t xml:space="preserve">study_domain_other :study_domain:!1,2</t>
+    <t xml:space="preserve">study_domain_other:study_domain:!1,2</t>
   </si>
   <si>
     <t xml:space="preserve">Veuillez également répondre à la question suivante :</t>
@@ -411,7 +411,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -432,11 +432,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -489,7 +484,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -499,10 +494,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -526,6 +517,112 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="LibreOffice">
+      <a:dk1>
+        <a:srgbClr val="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:srgbClr val="ffffff"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="000000"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="ffffff"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="18a303"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="0369a3"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="a33e03"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8e03a3"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="c99c00"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="c9211e"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000ee"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="551a8b"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Arial" pitchFamily="0" charset="1"/>
+        <a:ea typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+        <a:cs typeface="DejaVu Sans" pitchFamily="0" charset="1"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme>
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:prstDash val="solid"/>
+          <a:miter/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -534,7 +631,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I5" activeCellId="0" sqref="I5"/>
+      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -543,7 +640,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="13.75"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.22"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="22.22"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,7 +668,7 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="0" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -591,7 +688,7 @@
       <c r="E2" s="2" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
@@ -608,7 +705,7 @@
       <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>18</v>
       </c>
     </row>
@@ -622,7 +719,7 @@
       <c r="D4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="I4" s="2" t="s">
         <v>22</v>
       </c>
     </row>
@@ -673,7 +770,7 @@
       <c r="G7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H7" s="4"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -721,14 +818,13 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0" t="s">
+      <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -823,7 +919,7 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -861,7 +957,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -876,7 +972,7 @@
       <c r="E3" s="2" t="n">
         <v>12</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="4" t="s">
         <v>68</v>
       </c>
       <c r="G3" s="2" t="s">
@@ -899,7 +995,7 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -914,7 +1010,7 @@
       <c r="E4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="5"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="2" t="s">
         <v>72</v>
       </c>
@@ -929,7 +1025,7 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="4" t="s">
         <v>74</v>
       </c>
       <c r="B5" s="2" t="s">
@@ -941,7 +1037,7 @@
       <c r="D5" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="4" t="s">
         <v>75</v>
       </c>
       <c r="G5" s="2" t="s">
@@ -952,7 +1048,7 @@
       </c>
     </row>
     <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>78</v>
       </c>
       <c r="B6" s="2" t="s">
@@ -964,7 +1060,7 @@
       <c r="D6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>79</v>
       </c>
       <c r="G6" s="2" t="s">
@@ -975,7 +1071,7 @@
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>82</v>
       </c>
       <c r="B7" s="2" t="s">
@@ -995,7 +1091,7 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="4" t="s">
         <v>85</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1015,7 +1111,7 @@
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="4" t="s">
         <v>88</v>
       </c>
       <c r="B9" s="2" t="s">
@@ -1035,7 +1131,7 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="4" t="s">
         <v>91</v>
       </c>
       <c r="B10" s="2" t="s">
@@ -1055,7 +1151,7 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="4" t="s">
         <v>94</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1075,7 +1171,7 @@
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="4" t="s">
         <v>97</v>
       </c>
       <c r="B12" s="2" t="s">
@@ -1092,7 +1188,7 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="4" t="s">
         <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
@@ -1109,7 +1205,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>101</v>
       </c>
       <c r="B14" s="2" t="s">
@@ -1123,7 +1219,7 @@
       </c>
     </row>
     <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>102</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -1137,7 +1233,7 @@
       </c>
     </row>
     <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="4" t="s">
         <v>105</v>
       </c>
       <c r="B16" s="2" t="s">
@@ -1151,7 +1247,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="4" t="s">
         <v>107</v>
       </c>
       <c r="B17" s="2" t="s">
@@ -1165,7 +1261,7 @@
       </c>
     </row>
     <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="4" t="s">
         <v>108</v>
       </c>
       <c r="B18" s="2" t="s">
@@ -1179,7 +1275,7 @@
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="4" t="s">
         <v>109</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -1193,7 +1289,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="5" t="s">
+      <c r="A20" s="4" t="s">
         <v>110</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -1207,7 +1303,7 @@
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5" t="s">
+      <c r="A21" s="4" t="s">
         <v>111</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -1221,7 +1317,7 @@
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="5" t="s">
+      <c r="A22" s="4" t="s">
         <v>112</v>
       </c>
       <c r="B22" s="2" t="s">
@@ -1235,7 +1331,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="5" t="s">
+      <c r="A23" s="4" t="s">
         <v>113</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -1249,7 +1345,7 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="4" t="s">
         <v>114</v>
       </c>
       <c r="B24" s="2" t="s">

</xml_diff>

<commit_message>
correction leepquest.xlsx (french version)
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="116">
   <si>
     <t xml:space="preserve">LIST</t>
   </si>
@@ -268,6 +268,9 @@
     <t xml:space="preserve">Association nationale pour l’étude de la neige et des avalanches </t>
   </si>
   <si>
+    <t xml:space="preserve">Pour chacune des caractéristiques ou descriptions suivantes, indiquez à quel point chacune est vraie pour vous.</t>
+  </si>
+  <si>
     <t xml:space="preserve">asso_petitsprinces</t>
   </si>
   <si>
@@ -277,9 +280,6 @@
     <t xml:space="preserve">Association des petits princes</t>
   </si>
   <si>
-    <t xml:space="preserve">Sur une échelle de « 1 » (jamais) à « 5 » (souvent), répondez aux affirmations suivantes :</t>
-  </si>
-  <si>
     <t xml:space="preserve">asso_armeschasse</t>
   </si>
   <si>
@@ -287,9 +287,6 @@
   </si>
   <si>
     <t xml:space="preserve">Union nationale des propriétaires d’armes de chasse et de tir</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pour chacune des caractéristiques ou descriptions suivantes, indiquez à quel point chacune est vraie pour vous.</t>
   </si>
   <si>
     <t xml:space="preserve">asso_vehiculesepoque</t>
@@ -630,8 +627,8 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I3" activeCellId="0" sqref="I3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -860,8 +857,8 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M5" activeCellId="0" sqref="M5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -918,7 +915,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="46.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>59</v>
       </c>
@@ -956,7 +953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>65</v>
       </c>
@@ -994,7 +991,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
         <v>71</v>
       </c>
@@ -1010,12 +1007,14 @@
       <c r="E4" s="2" t="n">
         <v>10</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="G4" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="L4" s="1" t="n">
         <v>0</v>
@@ -1024,9 +1023,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>66</v>
@@ -1035,11 +1034,9 @@
         <v>67</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>75</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="F5" s="4"/>
       <c r="G5" s="2" t="s">
         <v>76</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>78</v>
       </c>
@@ -1060,19 +1057,17 @@
       <c r="D6" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="4" t="s">
+      <c r="F6" s="0"/>
+      <c r="G6" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="H6" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>81</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>66</v>
@@ -1081,18 +1076,18 @@
         <v>67</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>66</v>
@@ -1101,18 +1096,18 @@
         <v>67</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="G8" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>66</v>
@@ -1121,18 +1116,18 @@
         <v>67</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G9" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>66</v>
@@ -1141,18 +1136,18 @@
         <v>67</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>92</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>66</v>
@@ -1161,18 +1156,18 @@
         <v>67</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="G11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>66</v>
@@ -1181,15 +1176,15 @@
         <v>67</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>66</v>
@@ -1198,15 +1193,15 @@
         <v>67</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>66</v>
@@ -1215,60 +1210,60 @@
         <v>67</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="2" t="s">
         <v>103</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>104</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
         <v>107</v>
       </c>
-      <c r="B17" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="24.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>108</v>
-      </c>
       <c r="B18" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>77</v>
@@ -1276,86 +1271,86 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="4" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="B24" s="2" t="s">
-        <v>115</v>
-      </c>
       <c r="C24" s="2" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1384,7 +1379,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding possibility to desactivate tags in radio options' labels, rearanging columns in excel example
</commit_message>
<xml_diff>
--- a/leepquest/leepquest.xlsx
+++ b/leepquest/leepquest.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="A" sheetId="1" state="visible" r:id="rId3"/>
@@ -36,18 +36,18 @@
     <t xml:space="preserve">VARS</t>
   </si>
   <si>
+    <t xml:space="preserve">QUESTTAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">#HASTAGS</t>
+  </si>
+  <si>
     <t xml:space="preserve">BY</t>
   </si>
   <si>
     <t xml:space="preserve">BY_INTRO</t>
   </si>
   <si>
-    <t xml:space="preserve">HASTAGS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">QUESTTAG</t>
-  </si>
-  <si>
     <t xml:space="preserve">DEPS</t>
   </si>
   <si>
@@ -93,7 +93,7 @@
     <t xml:space="preserve">professional_status:student:2:inv</t>
   </si>
   <si>
-    <t xml:space="preserve">What is your gender?</t>
+    <t xml:space="preserve">What is your &lt;u&gt;gender&lt;/u&gt;?</t>
   </si>
   <si>
     <t xml:space="preserve">hradio</t>
@@ -105,9 +105,6 @@
     <t xml:space="preserve">genre</t>
   </si>
   <si>
-    <t xml:space="preserve">div style='font-size:120%'</t>
-  </si>
-  <si>
     <t xml:space="preserve">What is your country of birth?</t>
   </si>
   <si>
@@ -118,6 +115,9 @@
   </si>
   <si>
     <t xml:space="preserve">pays</t>
+  </si>
+  <si>
+    <t xml:space="preserve">div style='font-size:100%'</t>
   </si>
   <si>
     <r>
@@ -208,6 +208,12 @@
     <t xml:space="preserve">professional_status</t>
   </si>
   <si>
+    <t xml:space="preserve">MIN_TIMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PREV_BUTTONS</t>
+  </si>
+  <si>
     <t xml:space="preserve">ACTIVITIES_LIST</t>
   </si>
   <si>
@@ -221,12 +227,6 @@
   </si>
   <si>
     <t xml:space="preserve">#B_SAME_ORDERS_IN_ALL_ROUNDS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MIN_TIMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PREV_BUTTONS</t>
   </si>
   <si>
     <t xml:space="preserve">On a scale from 1 (very dissatisfied) to 5 (very satisfied), how satisfied are you with your current job?</t>
@@ -449,12 +449,14 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -518,35 +520,35 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -675,215 +677,220 @@
   </sheetPr>
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="80.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="36.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="80.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="41.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="10.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="10.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="11.39"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="C2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="G2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="0" t="s">
+      <c r="I2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="0" t="s">
+      <c r="I3" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="0" t="s">
+      <c r="I4" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="0" t="s">
+      <c r="D5" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H5" s="0" t="s">
+      <c r="E5" s="0"/>
+      <c r="F5" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="C6" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="0" t="s">
+      <c r="E6" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="C7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="D7" s="0" t="s">
+      <c r="D7" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="G7" s="0" t="n">
+      <c r="F7" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="G8" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B9" s="0" t="s">
+      <c r="B9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="C9" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="D9" s="0" t="s">
+      <c r="D9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="4" t="s">
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="0" t="s">
+      <c r="B10" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D10" s="0" t="s">
+      <c r="D10" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="4" t="s">
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="0" t="s">
+      <c r="B11" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="0" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="4" t="s">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B12" s="0" t="s">
+      <c r="B12" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D12" s="0" t="s">
+      <c r="D12" s="1" t="s">
         <v>51</v>
       </c>
     </row>
@@ -905,498 +912,499 @@
   </sheetPr>
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="48.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="51.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="79.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="31.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="32.74"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="48.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="51.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="79.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="11.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="15.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="25.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="15.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="31.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="32.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16380" style="0" width="11.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K2" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="L2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="M2" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G3" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="1" t="s">
+      <c r="H3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="E2" s="0" t="n">
+      <c r="L3" s="1" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="H4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="0" t="s">
+      <c r="I4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="I2" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="J2" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="K2" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L2" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="M2" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="F3" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="G3" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="H3" s="0" t="s">
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I3" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="J3" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L3" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="M3" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="E4" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="0" t="s">
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="L4" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M4" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>75</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="H5" s="0" t="s">
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>78</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D6" s="0" t="s">
-        <v>76</v>
-      </c>
-      <c r="G6" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="H6" s="0" t="s">
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="8" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C7" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D7" s="0" t="s">
-        <v>79</v>
-      </c>
-      <c r="G7" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="H7" s="0" t="s">
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
-        <v>84</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>82</v>
-      </c>
-      <c r="G8" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="H8" s="0" t="s">
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>85</v>
-      </c>
-      <c r="G9" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="H9" s="0" t="s">
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>90</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C10" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D10" s="0" t="s">
-        <v>88</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="H10" s="0" t="s">
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="8" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D23" s="1" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D11" s="0" t="s">
-        <v>91</v>
-      </c>
-      <c r="G11" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="H11" s="0" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>96</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C12" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>94</v>
-      </c>
-      <c r="G12" s="0" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>98</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C13" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D13" s="0" t="s">
-        <v>97</v>
-      </c>
-      <c r="G13" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>100</v>
-      </c>
-      <c r="B14" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="C14" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="0" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>101</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="2" t="s">
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="B16" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D16" s="0" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="B17" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D17" s="0" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="B18" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C18" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D18" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D19" s="0" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D20" s="0" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="B21" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D21" s="0" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="B22" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D22" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="7" t="s">
-        <v>112</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>105</v>
-      </c>
-      <c r="C23" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D23" s="0" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
-        <v>113</v>
-      </c>
-      <c r="B24" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="D24" s="0" t="s">
+      <c r="D24" s="1" t="s">
         <v>95</v>
       </c>
     </row>
@@ -1425,7 +1433,7 @@
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="3" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>